<commit_message>
Update 0.6 : tasklist & viewPost
Bug fix:
fix
createPost btAction

Reconstruct :
postTbl

Task list:
+createVote.jsp -> Create vote -> post -> viewPost -> btAction="User_Vote"
UserVoteServlet -> viewPost.jsp

+image input Filechooser or String http

+css <3
</commit_message>
<xml_diff>
--- a/Database_G2_Forum_update3.xlsx
+++ b/Database_G2_Forum_update3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APC\Desktop\G2ForumWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F744A47-D0AA-469E-B3A8-35429AC9266E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6626D7B-914D-4AB0-A44F-BA511DAA8A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{43A04236-E20D-42A3-B2D5-0D9A3173A71B}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="148">
   <si>
     <t>G2ForumWeb Database</t>
   </si>
@@ -322,9 +322,6 @@
     <t>topic_id**</t>
   </si>
   <si>
-    <t>(1 = up,- 1 = down)</t>
-  </si>
-  <si>
     <t>topicTbl</t>
   </si>
   <si>
@@ -404,6 +401,78 @@
   </si>
   <si>
     <t>ViewPost.jsp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  =comment_id</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>comment Of comment</t>
+  </si>
+  <si>
+    <t>cateloryID</t>
+  </si>
+  <si>
+    <t>type_id</t>
+  </si>
+  <si>
+    <t>(1 = up, - 1 = down)</t>
+  </si>
+  <si>
+    <t>(3) &gt; modViewVote.jsp</t>
+  </si>
+  <si>
+    <t>vote_type sum</t>
+  </si>
+  <si>
+    <t>isApprove = mod_id != null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 - 1 </t>
+  </si>
+  <si>
+    <t>mod_id - null - int</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>Create Vote = Post</t>
+  </si>
+  <si>
+    <t>Vote - vote func DAO</t>
+  </si>
+  <si>
+    <t>Post -&gt; Vote</t>
+  </si>
+  <si>
+    <t>VoteTbl = post_id</t>
+  </si>
+  <si>
+    <t>Mod -&gt; View Vote -&gt; approve by isHidden</t>
+  </si>
+  <si>
+    <t>ApproveAble -&gt; vote_type sum = 3;</t>
+  </si>
+  <si>
+    <t>func vote_type Sum all votetype by post_id</t>
+  </si>
+  <si>
+    <t>user &gt;- vote</t>
+  </si>
+  <si>
+    <t>vote id -&gt; post_id</t>
+  </si>
+  <si>
+    <t>checkDub vote :</t>
+  </si>
+  <si>
+    <t>vote id -&gt; post_id AND create_user_id ==  get user.id</t>
+  </si>
+  <si>
+    <t>voteSum</t>
   </si>
 </sst>
 </file>
@@ -681,7 +750,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
@@ -728,6 +797,18 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -740,19 +821,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
@@ -761,7 +839,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
@@ -770,15 +848,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent5" xfId="3" builtinId="47"/>
@@ -1912,20 +1982,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170864F1-DF9A-4B54-B6E4-0541A319C080}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.21875" customWidth="1"/>
     <col min="4" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1933,6 +2002,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+    </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -1946,11 +2035,14 @@
         <v>66</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>78</v>
       </c>
@@ -1964,16 +2056,19 @@
         <v>2</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2017,6 +2112,9 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>138</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
@@ -2034,6 +2132,9 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2065,6 +2166,9 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>75</v>
       </c>
@@ -2079,6 +2183,9 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>141</v>
+      </c>
       <c r="C15" s="5" t="s">
         <v>76</v>
       </c>
@@ -2093,14 +2200,23 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C17" s="7" t="s">
         <v>71</v>
       </c>
@@ -2114,7 +2230,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C18" s="8" t="s">
         <v>68</v>
       </c>
@@ -2122,7 +2238,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
         <v>48</v>
       </c>
@@ -2132,7 +2248,10 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>133</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>79</v>
       </c>
@@ -2145,8 +2264,20 @@
       <c r="G20" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>125</v>
+      </c>
+      <c r="K20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>86</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
@@ -2163,7 +2294,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>132</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>57</v>
       </c>
@@ -2179,8 +2313,17 @@
       <c r="G22" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="J22" t="s">
+        <v>125</v>
+      </c>
+      <c r="L22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>67</v>
       </c>
@@ -2194,9 +2337,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" t="s">
+        <v>135</v>
+      </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>22</v>
@@ -2205,15 +2354,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E25" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>124</v>
+      </c>
+      <c r="J25" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2226,7 +2381,7 @@
   <dimension ref="A2:AC35"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD23" sqref="AD23"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2246,13 +2401,13 @@
         <v>59</v>
       </c>
       <c r="O2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U2" t="s">
         <v>110</v>
       </c>
-      <c r="U2" t="s">
-        <v>111</v>
-      </c>
       <c r="AA2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
@@ -2327,97 +2482,97 @@
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="G6" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K6" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N6" s="15"/>
       <c r="O6" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T6" s="15"/>
       <c r="U6" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="V6" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="W6" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Y6" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Z6" s="15"/>
       <c r="AA6" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB6" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AC6" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G7" s="24"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
-      <c r="J7" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="K7" s="30"/>
+      <c r="J7" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="K7" s="40"/>
       <c r="M7" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="N7" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="O7" s="30"/>
-      <c r="P7" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q7" s="30"/>
+        <v>117</v>
+      </c>
+      <c r="N7" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="O7" s="40"/>
+      <c r="P7" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q7" s="40"/>
       <c r="S7" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="T7" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="U7" s="30"/>
-      <c r="V7" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="W7" s="30"/>
+        <v>117</v>
+      </c>
+      <c r="T7" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="U7" s="40"/>
+      <c r="V7" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="W7" s="40"/>
       <c r="Y7" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z7" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA7" s="30"/>
-      <c r="AB7" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC7" s="30"/>
+        <v>117</v>
+      </c>
+      <c r="Z7" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA7" s="40"/>
+      <c r="AB7" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC7" s="40"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2426,306 +2581,306 @@
       <c r="D8" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="M8" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="31"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="41"/>
       <c r="Q8" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="S8" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="S8" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="31"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="41"/>
       <c r="W8" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y8" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y8" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="Z8" s="35"/>
-      <c r="AA8" s="35"/>
-      <c r="AB8" s="35"/>
+      <c r="Z8" s="45"/>
+      <c r="AA8" s="45"/>
+      <c r="AB8" s="45"/>
       <c r="AC8" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="30"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="M9" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="M9" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="30"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="40"/>
       <c r="Q9" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="S9" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="S9" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="30"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="40"/>
       <c r="W9" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y9" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y9" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="Z9" s="35"/>
-      <c r="AA9" s="35"/>
-      <c r="AB9" s="35"/>
+      <c r="Z9" s="45"/>
+      <c r="AA9" s="45"/>
+      <c r="AB9" s="45"/>
       <c r="AC9" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="30"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="M10" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="M10" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="30"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="40"/>
       <c r="Q10" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="S10" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="S10" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="30"/>
+      <c r="T10" s="39"/>
+      <c r="U10" s="39"/>
+      <c r="V10" s="40"/>
       <c r="W10" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y10" s="40"/>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="41"/>
-      <c r="AB10" s="41"/>
+        <v>106</v>
+      </c>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="50"/>
+      <c r="AA10" s="50"/>
+      <c r="AB10" s="50"/>
       <c r="AC10" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="M11" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="M11" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="30"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="40"/>
       <c r="Q11" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="S11" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="S11" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="30"/>
+      <c r="T11" s="39"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="40"/>
       <c r="W11" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y11" s="32"/>
-      <c r="Z11" s="35"/>
-      <c r="AA11" s="35"/>
-      <c r="AB11" s="35"/>
+        <v>106</v>
+      </c>
+      <c r="Y11" s="44"/>
+      <c r="Z11" s="45"/>
+      <c r="AA11" s="45"/>
+      <c r="AB11" s="45"/>
       <c r="AC11" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="30"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40"/>
       <c r="K12" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="M12" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="M12" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="30"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="40"/>
       <c r="Q12" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="S12" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="S12" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="30"/>
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="40"/>
       <c r="W12" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y12" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y12" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z12" s="42"/>
+      <c r="AA12" s="42"/>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G13" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="M13" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="S13" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="T13" s="39"/>
+      <c r="U13" s="39"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y13" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z13" s="42"/>
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="43"/>
+      <c r="AC13" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G14" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="M14" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="S14" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="T14" s="39"/>
+      <c r="U14" s="39"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y14" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z14" s="42"/>
+      <c r="AA14" s="42"/>
+      <c r="AB14" s="43"/>
+      <c r="AC14" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G15" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="M15" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="S15" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="T15" s="39"/>
+      <c r="U15" s="39"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y15" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="Z12" s="36"/>
-      <c r="AA12" s="36"/>
-      <c r="AB12" s="34"/>
-      <c r="AC12" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="G13" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="M13" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="S13" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y13" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z13" s="36"/>
-      <c r="AA13" s="36"/>
-      <c r="AB13" s="34"/>
-      <c r="AC13" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="G14" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="M14" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="S14" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="T14" s="29"/>
-      <c r="U14" s="29"/>
-      <c r="V14" s="30"/>
-      <c r="W14" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y14" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z14" s="36"/>
-      <c r="AA14" s="36"/>
-      <c r="AB14" s="34"/>
-      <c r="AC14" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="G15" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="M15" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="S15" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y15" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="Z15" s="38"/>
-      <c r="AA15" s="38"/>
-      <c r="AB15" s="31"/>
+      <c r="Z15" s="47"/>
+      <c r="AA15" s="47"/>
+      <c r="AB15" s="41"/>
       <c r="AC15" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
@@ -2774,13 +2929,13 @@
     </row>
     <row r="20" spans="7:29" x14ac:dyDescent="0.3">
       <c r="I20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="7:29" x14ac:dyDescent="0.3">
@@ -2851,264 +3006,264 @@
     </row>
     <row r="24" spans="7:29" x14ac:dyDescent="0.3">
       <c r="G24" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T24" s="15"/>
       <c r="U24" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="V24" s="15"/>
       <c r="W24" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Y24" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Z24" s="15"/>
       <c r="AA24" s="15"/>
       <c r="AB24" s="15"/>
       <c r="AC24" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="7:29" x14ac:dyDescent="0.3">
       <c r="G25" s="16"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="34"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="43"/>
       <c r="M25" s="16"/>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="34"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="43"/>
       <c r="S25" s="16"/>
       <c r="T25" s="14"/>
       <c r="U25" s="14"/>
-      <c r="V25" s="36"/>
-      <c r="W25" s="34"/>
+      <c r="V25" s="42"/>
+      <c r="W25" s="43"/>
       <c r="Y25" s="16"/>
       <c r="Z25" s="14"/>
       <c r="AA25" s="14"/>
-      <c r="AB25" s="36"/>
-      <c r="AC25" s="34"/>
+      <c r="AB25" s="42"/>
+      <c r="AC25" s="43"/>
     </row>
     <row r="26" spans="7:29" x14ac:dyDescent="0.3">
-      <c r="G26" s="42"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="39"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="48"/>
-      <c r="Q26" s="39"/>
-      <c r="S26" s="42"/>
-      <c r="T26" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="U26" s="47"/>
-      <c r="V26" s="48"/>
-      <c r="W26" s="39"/>
-      <c r="Y26" s="42"/>
-      <c r="Z26" s="46"/>
-      <c r="AA26" s="47"/>
-      <c r="AB26" s="48"/>
-      <c r="AC26" s="39"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="28"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="28"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="U26" s="34"/>
+      <c r="V26" s="35"/>
+      <c r="W26" s="28"/>
+      <c r="Y26" s="29"/>
+      <c r="Z26" s="33"/>
+      <c r="AA26" s="34"/>
+      <c r="AB26" s="35"/>
+      <c r="AC26" s="28"/>
     </row>
     <row r="27" spans="7:29" x14ac:dyDescent="0.3">
-      <c r="G27" s="42"/>
-      <c r="H27" s="42" t="s">
+      <c r="G27" s="29"/>
+      <c r="H27" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="I27" s="30"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="20"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="O27" s="30"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="20"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="U27" s="30"/>
+      <c r="V27" s="36"/>
+      <c r="W27" s="20"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA27" s="30"/>
+      <c r="AB27" s="36"/>
+      <c r="AC27" s="20"/>
+    </row>
+    <row r="28" spans="7:29" x14ac:dyDescent="0.3">
+      <c r="G28" s="29"/>
+      <c r="H28" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="I27" s="43"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="20"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42" t="s">
+      <c r="I28" s="30"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="20"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="O27" s="43"/>
-      <c r="P27" s="49"/>
-      <c r="Q27" s="20"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="U27" s="43"/>
-      <c r="V27" s="49"/>
-      <c r="W27" s="20"/>
-      <c r="Y27" s="42"/>
-      <c r="Z27" s="42" t="s">
+      <c r="O28" s="30"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="20"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="U28" s="30"/>
+      <c r="V28" s="36"/>
+      <c r="W28" s="20"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="AA27" s="43"/>
-      <c r="AB27" s="49"/>
-      <c r="AC27" s="20"/>
-    </row>
-    <row r="28" spans="7:29" x14ac:dyDescent="0.3">
-      <c r="G28" s="42"/>
-      <c r="H28" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="I28" s="43"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="20"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="O28" s="43"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="20"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="U28" s="43"/>
-      <c r="V28" s="49"/>
-      <c r="W28" s="20"/>
-      <c r="Y28" s="42"/>
-      <c r="Z28" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA28" s="43"/>
-      <c r="AB28" s="49"/>
+      <c r="AA28" s="30"/>
+      <c r="AB28" s="36"/>
       <c r="AC28" s="20"/>
     </row>
     <row r="29" spans="7:29" x14ac:dyDescent="0.3">
-      <c r="G29" s="42"/>
-      <c r="H29" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="I29" s="43"/>
-      <c r="J29" s="49"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="I29" s="30"/>
+      <c r="J29" s="36"/>
       <c r="K29" s="20"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="49"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="36"/>
       <c r="Q29" s="20"/>
-      <c r="S29" s="42"/>
-      <c r="T29" s="42"/>
-      <c r="U29" s="43"/>
-      <c r="V29" s="49"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="29"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="36"/>
       <c r="W29" s="20"/>
-      <c r="Y29" s="42"/>
-      <c r="Z29" s="42"/>
-      <c r="AA29" s="43"/>
-      <c r="AB29" s="49"/>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="29"/>
+      <c r="AA29" s="30"/>
+      <c r="AB29" s="36"/>
       <c r="AC29" s="20"/>
     </row>
     <row r="30" spans="7:29" x14ac:dyDescent="0.3">
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="49"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="36"/>
       <c r="K30" s="20"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="49"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="36"/>
       <c r="Q30" s="20"/>
-      <c r="S30" s="42"/>
-      <c r="T30" s="42"/>
-      <c r="U30" s="43"/>
-      <c r="V30" s="49"/>
+      <c r="S30" s="29"/>
+      <c r="T30" s="29"/>
+      <c r="U30" s="30"/>
+      <c r="V30" s="36"/>
       <c r="W30" s="20"/>
-      <c r="Y30" s="42"/>
-      <c r="Z30" s="42"/>
-      <c r="AA30" s="43"/>
-      <c r="AB30" s="49"/>
+      <c r="Y30" s="29"/>
+      <c r="Z30" s="29"/>
+      <c r="AA30" s="30"/>
+      <c r="AB30" s="36"/>
       <c r="AC30" s="20"/>
     </row>
     <row r="31" spans="7:29" x14ac:dyDescent="0.3">
-      <c r="G31" s="42"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="50"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="37"/>
       <c r="K31" s="20"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="50"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="37"/>
       <c r="Q31" s="20"/>
-      <c r="S31" s="42"/>
-      <c r="T31" s="42" t="s">
+      <c r="S31" s="29"/>
+      <c r="T31" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="U31" s="43"/>
-      <c r="V31" s="49"/>
+      <c r="U31" s="30"/>
+      <c r="V31" s="36"/>
       <c r="W31" s="20"/>
-      <c r="Y31" s="42"/>
-      <c r="Z31" s="44"/>
-      <c r="AA31" s="45"/>
-      <c r="AB31" s="50"/>
+      <c r="Y31" s="29"/>
+      <c r="Z31" s="31"/>
+      <c r="AA31" s="32"/>
+      <c r="AB31" s="37"/>
       <c r="AC31" s="20"/>
     </row>
     <row r="32" spans="7:29" x14ac:dyDescent="0.3">
-      <c r="G32" s="32"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
       <c r="K32" s="20"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="43"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
       <c r="Q32" s="20"/>
-      <c r="S32" s="42"/>
-      <c r="T32" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="U32" s="45"/>
-      <c r="V32" s="50"/>
+      <c r="S32" s="29"/>
+      <c r="T32" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="U32" s="32"/>
+      <c r="V32" s="37"/>
       <c r="W32" s="20"/>
-      <c r="Y32" s="42"/>
-      <c r="Z32" s="43"/>
-      <c r="AA32" s="43"/>
-      <c r="AB32" s="43"/>
+      <c r="Y32" s="29"/>
+      <c r="Z32" s="30"/>
+      <c r="AA32" s="30"/>
+      <c r="AB32" s="30"/>
       <c r="AC32" s="20"/>
     </row>
     <row r="33" spans="7:29" x14ac:dyDescent="0.3">
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
       <c r="K33" s="23"/>
-      <c r="M33" s="44"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
       <c r="Q33" s="23"/>
-      <c r="S33" s="44"/>
-      <c r="T33" s="45"/>
-      <c r="U33" s="45"/>
-      <c r="V33" s="45"/>
+      <c r="S33" s="31"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
       <c r="W33" s="23"/>
-      <c r="Y33" s="44"/>
-      <c r="Z33" s="45"/>
-      <c r="AA33" s="45"/>
-      <c r="AB33" s="45"/>
+      <c r="Y33" s="31"/>
+      <c r="Z33" s="32"/>
+      <c r="AA33" s="32"/>
+      <c r="AB33" s="32"/>
       <c r="AC33" s="23"/>
     </row>
     <row r="34" spans="7:29" x14ac:dyDescent="0.3">
@@ -3157,17 +3312,16 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="T7:U7"/>
     <mergeCell ref="AB7:AC7"/>
     <mergeCell ref="Y8:AB8"/>
     <mergeCell ref="Y9:AB9"/>
     <mergeCell ref="Y10:AB10"/>
+    <mergeCell ref="Z7:AA7"/>
     <mergeCell ref="Y11:AB11"/>
     <mergeCell ref="Y12:AB12"/>
     <mergeCell ref="Y13:AB13"/>
     <mergeCell ref="Y14:AB14"/>
     <mergeCell ref="Y15:AB15"/>
-    <mergeCell ref="Z7:AA7"/>
     <mergeCell ref="AB25:AC25"/>
     <mergeCell ref="V25:W25"/>
     <mergeCell ref="J25:K25"/>
@@ -3183,6 +3337,7 @@
     <mergeCell ref="S9:V9"/>
     <mergeCell ref="S10:V10"/>
     <mergeCell ref="S11:V11"/>
+    <mergeCell ref="T7:U7"/>
     <mergeCell ref="M11:P11"/>
     <mergeCell ref="M12:P12"/>
     <mergeCell ref="G8:J8"/>

</xml_diff>